<commit_message>
Auslegung Schmelzsicherung & Bestellliste hinzugefügt
</commit_message>
<xml_diff>
--- a/5. Dokumente/Datenmodell.xlsx
+++ b/5. Dokumente/Datenmodell.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1. Eigene Dateien\1. Studium\2. Staatliches Studium\HTW Berlin\2. Masterstudium\1. Hochschulskripte\2. SoSe 2022\VA2 Hochverfügbare und sichere Systeme\2. Belegaufgabe\Belegarbeit-Hochverfuegbare-Systeme\5. Dokumente\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0115E1DF-256C-45DB-89CB-7D579A1223B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Datenmodell" sheetId="1" r:id="rId4"/>
+    <sheet name="Datenmodell" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjp3IazpaMBY6uMYDBa36zbNVCbyQ=="/>
@@ -219,34 +228,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -256,7 +268,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -272,59 +284,65 @@
     </fill>
   </fills>
   <borders count="23">
-    <border/>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -333,17 +351,44 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -358,8 +403,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -369,27 +416,34 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -399,6 +453,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -413,27 +468,38 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -442,19 +508,29 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -463,179 +539,184 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="60">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -825,597 +906,644 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:N1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="9.14"/>
-    <col customWidth="1" min="3" max="3" width="10.57"/>
-    <col customWidth="1" min="4" max="6" width="9.71"/>
-    <col customWidth="1" min="7" max="7" width="19.71"/>
-    <col customWidth="1" min="8" max="10" width="9.14"/>
-    <col customWidth="1" min="11" max="14" width="10.71"/>
-    <col customWidth="1" min="15" max="26" width="9.14"/>
+    <col min="1" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="6" width="9.7265625" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" customWidth="1"/>
+    <col min="8" max="10" width="9.08984375" customWidth="1"/>
+    <col min="11" max="14" width="10.7265625" customWidth="1"/>
+    <col min="15" max="26" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:14" ht="14.5">
+      <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="2" t="s">
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
     </row>
-    <row r="4">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="6"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10" t="s">
+    <row r="4" spans="2:14" ht="14.5">
+      <c r="B4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="13"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16" t="s">
+    <row r="5" spans="2:14" ht="14.5">
+      <c r="B5" s="5"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="17"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7"/>
     </row>
-    <row r="6">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20" t="s">
+    <row r="6" spans="2:14" ht="14.5">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="42"/>
     </row>
-    <row r="7">
-      <c r="B7" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="C7" s="24" t="s">
+    <row r="7" spans="2:14" ht="14.5">
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="25" t="s">
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="26" t="s">
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="29"/>
+      <c r="N7" s="15"/>
     </row>
-    <row r="8">
-      <c r="B8" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="C8" s="30" t="s">
+    <row r="8" spans="2:14" ht="14.5">
+      <c r="B8" s="11">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="25" t="s">
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="26" t="s">
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="32" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="C9" s="24" t="s">
+    <row r="9" spans="2:14" ht="14.5">
+      <c r="B9" s="16">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="25" t="s">
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="26" t="s">
+      <c r="I9" s="44"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="32" t="s">
+      <c r="L9" s="13"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="30">
-        <v>4.0</v>
-      </c>
-      <c r="C10" s="24" t="s">
+    <row r="10" spans="2:14" ht="14.5">
+      <c r="B10" s="16">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="25" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="26" t="s">
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="32" t="s">
+      <c r="L10" s="13"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="30">
-        <v>5.0</v>
-      </c>
-      <c r="C11" s="24" t="s">
+    <row r="11" spans="2:14" ht="14.5">
+      <c r="B11" s="16">
+        <v>5</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="25" t="s">
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="26" t="s">
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="32" t="s">
+      <c r="L11" s="13"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="13"/>
-      <c r="C12" s="33" t="s">
+    <row r="12" spans="2:14" ht="14.5">
+      <c r="B12" s="5"/>
+      <c r="C12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="4"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="48"/>
     </row>
-    <row r="13">
-      <c r="B13" s="35">
-        <v>6.0</v>
-      </c>
-      <c r="C13" s="24" t="s">
+    <row r="13" spans="2:14" ht="14.5">
+      <c r="B13" s="20">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="36" t="s">
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="37" t="s">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="39" t="s">
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="35">
-        <v>7.0</v>
-      </c>
-      <c r="C14" s="24" t="s">
+    <row r="14" spans="2:14" ht="14.5">
+      <c r="B14" s="20">
+        <v>7</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="25" t="s">
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="40" t="s">
+      <c r="I14" s="44"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42" t="s">
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="35">
-        <v>8.0</v>
-      </c>
-      <c r="C15" s="24" t="s">
+    <row r="15" spans="2:14" ht="14.5">
+      <c r="B15" s="20">
+        <v>8</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="25" t="s">
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="40" t="s">
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="C16" s="24" t="s">
+    <row r="16" spans="2:14" ht="14.5">
+      <c r="B16" s="11">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="25" t="s">
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="26" t="s">
+      <c r="I16" s="44"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="32" t="s">
+      <c r="L16" s="13"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="24">
-        <v>10.0</v>
-      </c>
-      <c r="C17" s="24" t="s">
+    <row r="17" spans="2:14" ht="14.5">
+      <c r="B17" s="11">
+        <v>10</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="25" t="s">
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="26" t="s">
+      <c r="I17" s="44"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="43" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="44"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="45"/>
+    <row r="18" spans="2:14" ht="14.5">
+      <c r="B18" s="57"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="58"/>
     </row>
-    <row r="19">
-      <c r="B19" s="30"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="16" t="s">
+    <row r="19" spans="2:14" ht="14.5">
+      <c r="B19" s="16"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="48"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="30"/>
     </row>
-    <row r="20">
-      <c r="B20" s="50"/>
-      <c r="C20" s="51" t="s">
+    <row r="20" spans="2:14" ht="14.5">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="23"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="42"/>
     </row>
-    <row r="21">
-      <c r="B21" s="24">
-        <v>11.0</v>
-      </c>
-      <c r="C21" s="24" t="s">
+    <row r="21" spans="2:14" ht="14.5">
+      <c r="B21" s="11">
+        <v>11</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="25" t="s">
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="26" t="s">
+      <c r="I21" s="44"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="M21" s="28" t="s">
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="43" t="s">
+      <c r="N21" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22">
-      <c r="B22" s="24">
-        <v>12.0</v>
-      </c>
-      <c r="C22" s="24" t="s">
+    <row r="22" spans="2:14" ht="14.5">
+      <c r="B22" s="11">
+        <v>12</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="25" t="s">
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="26" t="s">
+      <c r="I22" s="44"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L22" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="M22" s="52" t="s">
+      <c r="L22" s="11">
+        <v>2</v>
+      </c>
+      <c r="M22" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="N22" s="43" t="s">
+      <c r="N22" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" s="24">
-        <v>13.0</v>
-      </c>
-      <c r="C23" s="24" t="s">
+    <row r="23" spans="2:14" ht="14.5">
+      <c r="B23" s="11">
+        <v>13</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="25" t="s">
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="26" t="s">
+      <c r="I23" s="44"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L23" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="M23" s="52" t="s">
+      <c r="L23" s="11">
+        <v>3</v>
+      </c>
+      <c r="M23" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="43" t="s">
+      <c r="N23" s="27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" s="50"/>
-      <c r="C24" s="20" t="s">
+    <row r="24" spans="2:14" ht="14.5">
+      <c r="B24" s="32"/>
+      <c r="C24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="45"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="58"/>
     </row>
-    <row r="25">
-      <c r="B25" s="24">
-        <v>14.0</v>
-      </c>
-      <c r="C25" s="24" t="s">
+    <row r="25" spans="2:14" ht="14.5">
+      <c r="B25" s="11">
+        <v>14</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="25" t="s">
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="26" t="s">
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="27"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="32" t="s">
+      <c r="L25" s="13"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="24">
-        <v>16.0</v>
-      </c>
-      <c r="C26" s="24" t="s">
+    <row r="26" spans="2:14" ht="14.5">
+      <c r="B26" s="11">
+        <v>16</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="25" t="s">
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="26" t="s">
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="27"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32" t="s">
+      <c r="L26" s="13"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27">
-      <c r="B27" s="19">
-        <v>17.0</v>
-      </c>
-      <c r="C27" s="19" t="s">
+    <row r="27" spans="2:14" ht="14.5">
+      <c r="B27" s="9">
+        <v>17</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="54" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="55" t="s">
+      <c r="I27" s="41"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L27" s="56"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="57" t="s">
+      <c r="L27" s="36"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="28" spans="2:14" ht="15.75" customHeight="1"/>
+    <row r="29" spans="2:14" ht="15.75" customHeight="1"/>
+    <row r="30" spans="2:14" ht="15.75" customHeight="1"/>
+    <row r="31" spans="2:14" ht="15.75" customHeight="1"/>
+    <row r="32" spans="2:14" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2393,39 +2521,6 @@
     <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:N6"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="D12:N12"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:G4"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="B18:N18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D20:N20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="D25:G25"/>
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="D27:G27"/>
@@ -2437,13 +2532,44 @@
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="D24:N24"/>
     <mergeCell ref="H25:J25"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="D20:N20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="B18:N18"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:J15"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:G4"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>